<commit_message>
Updated with test case information
</commit_message>
<xml_diff>
--- a/tests/test_cases.xlsx
+++ b/tests/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\peleke\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tprid\OneDrive\Desktop\Internship_BetterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E7FC38-D3E8-42E8-A6EA-CADB401272C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12382831-4707-412F-94DA-ED635BF9BEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_cases" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
   <si>
     <t>pdb_id</t>
   </si>
@@ -154,13 +154,175 @@
   </si>
   <si>
     <t>DIQMTQSPSSLSASVGDRVTITCRASQSISTHLNWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPWTFGQGTKVEIKRTVAAPSVFIFPPSDEQLKSGTASVVCLLNNFYPREAKVQWKVDNALQSGNSQESVTEQDSKDSTYSLSSTLTLSKADYEKHKVYACEVTHQGLSSPVTKSFNRGE</t>
+  </si>
+  <si>
+    <t>ma-1dqrd</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-c7d6n</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-cjnxd</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-cdl3l</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-cru5u</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-ci9yk</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-c8s4s</t>
+  </si>
+  <si>
+    <t>https://www.modelarchive.org/doi/10.5452/ma-1dqrd</t>
+  </si>
+  <si>
+    <t>https://www.rcsb.org/structure/2WH6</t>
+  </si>
+  <si>
+    <t>https://www.rcsb.org/structure/8HGO</t>
+  </si>
+  <si>
+    <t>https://www.rcsb.org/structure/4OO8</t>
+  </si>
+  <si>
+    <t>https://www.rcsb.org/structure/3DI3</t>
+  </si>
+  <si>
+    <t>https://www.rcsb.org/structure/1PEB</t>
+  </si>
+  <si>
+    <t>https://www.rcsb.org/structure/4Z18</t>
+  </si>
+  <si>
+    <t>Antigen type</t>
+  </si>
+  <si>
+    <t>Antigen source</t>
+  </si>
+  <si>
+    <t>Antigen name</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>human</t>
+  </si>
+  <si>
+    <t>lysozyme</t>
+  </si>
+  <si>
+    <t>ma-dpr9i (7u2e)</t>
+  </si>
+  <si>
+    <t>virus</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 receptor binding domain</t>
+  </si>
+  <si>
+    <t>ma-cdl3l (2EXP)</t>
+  </si>
+  <si>
+    <t>EGFR peptide</t>
+  </si>
+  <si>
+    <t>protein(peptide)</t>
+  </si>
+  <si>
+    <t>ma-cjnxd (1OSO)</t>
+  </si>
+  <si>
+    <t>bacteria</t>
+  </si>
+  <si>
+    <t>ma-c7d6n (1HFM)</t>
+  </si>
+  <si>
+    <t>ma-cru5u (1EM4)</t>
+  </si>
+  <si>
+    <t>ma-ci9yk (1ATM)</t>
+  </si>
+  <si>
+    <t>ma-c8s4s(1IIF)</t>
+  </si>
+  <si>
+    <t>HY/HEL-10 FAB-LYSOZYME </t>
+  </si>
+  <si>
+    <t>Not sure, here is pupmed link to article:https://pubmed.ncbi.nlm.nih.gov/12818205/</t>
+  </si>
+  <si>
+    <t>Benzo[A]pyrene</t>
+  </si>
+  <si>
+    <t>polycylic aromatic hydrocarbon(pah)</t>
+  </si>
+  <si>
+    <t>environmental</t>
+  </si>
+  <si>
+    <t>glycoprotein</t>
+  </si>
+  <si>
+    <t>Ley tetrasaccharide</t>
+  </si>
+  <si>
+    <t>p24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virus </t>
+  </si>
+  <si>
+    <t>BH3 peptide</t>
+  </si>
+  <si>
+    <t>EGFR/HER2 ectodomain</t>
+  </si>
+  <si>
+    <t>glycosylated human interleukin-7 receptor alpha ectodomain</t>
+  </si>
+  <si>
+    <t>endonuclease</t>
+  </si>
+  <si>
+    <t>BHRF1 (2WH6)</t>
+  </si>
+  <si>
+    <t>EGFR (8HGO0</t>
+  </si>
+  <si>
+    <t>Cas9 (4OO8)</t>
+  </si>
+  <si>
+    <t>IL-7Ra (3DI3)</t>
+  </si>
+  <si>
+    <t>maltose</t>
+  </si>
+  <si>
+    <t>carbohydrate</t>
+  </si>
+  <si>
+    <t>MBP (1PEB)</t>
+  </si>
+  <si>
+    <t>programmed cell death ligand 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -175,6 +337,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,6 +388,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -613,128 +811,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="7" max="7" width="37.375" customWidth="1"/>
-    <col min="8" max="8" width="45.875" customWidth="1"/>
-    <col min="9" max="9" width="52.625" customWidth="1"/>
-    <col min="10" max="10" width="45.5" customWidth="1"/>
+    <col min="3" max="5" width="47" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="10.58203125" customWidth="1"/>
+    <col min="9" max="9" width="38" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" customWidth="1"/>
+    <col min="11" max="11" width="45.83203125" customWidth="1"/>
+    <col min="12" max="12" width="52.58203125" customWidth="1"/>
+    <col min="13" max="13" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="str">
-        <f>_xlfn.CONCAT(F2,"|",G2)</f>
+      <c r="L2" s="2" t="str">
+        <f>_xlfn.CONCAT(I2,"|",J2)</f>
         <v>DVQLQESGPSLVKPSQTLSLTCSVTGDSITSDYWSWIRKFPGNRLEYMGYVSYSGSTYYNPSLKSRISITRDTSKNQYYLDLNSVTTEDTATYYCANWDGDYWGQGTLVTVSA|DIVLTQSPATLSVTPGNSVSLSCRASQSIGNNLHWYQQKSHESPRLLIKYASQSISGIPSRFSGSGSGTDFTLSINSVETEDFGMYFCQQSNSWPYTFGGGTKLEIK</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f>_xlfn.CONCAT(F3,"|",G3)</f>
+      <c r="L3" s="2" t="str">
+        <f>_xlfn.CONCAT(I3,"|",J3)</f>
         <v>DVQLQESGPSLVKPSQTLSLTCSVTGDSITSDYWSWIRKFPGNRLEYMGYVSYSGSTYYNPSLKSRISITRDTSKNQYYLDLNSVTTEDTATYYCANWDGDYWGQGTLVTVSA|DIVLTQSPATLSVTPGNSVSLSCRASQSIGNNLHWYQQKSHESPRLLIKYASQSISGIPSRFSGSGSGTDFTLSINSVETEDFGMYFCQQSNSWPYTFGGGTKLEIK</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{7D222CE2-D492-4B26-BAA3-242612EB0D78}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{96D64327-D74D-41F4-AB50-E666F553F258}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{DC808CB5-B7AF-4205-A1A6-896778A70EF3}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{F6672930-47AC-46D7-8558-3ACBA9AFD7D7}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{6A84F481-8B5A-4389-9A71-5326690E04E5}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{FC09CDCA-BC25-4CAF-B291-183DEF835D47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -749,7 +1200,7 @@
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="9" style="3"/>
     <col min="3" max="3" width="62.75" style="4" customWidth="1"/>
@@ -757,7 +1208,7 @@
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -771,7 +1222,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -785,7 +1236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -799,7 +1250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -813,7 +1264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -827,7 +1278,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -841,7 +1292,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Update to include antigen seqs
</commit_message>
<xml_diff>
--- a/tests/test_cases.xlsx
+++ b/tests/test_cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tprid\OneDrive\Desktop\Internship_BetterData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4536a64ec9700c3e/Desktop/Internship_BetterData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12382831-4707-412F-94DA-ED635BF9BEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0A2A072-429D-4010-9102-BE5A85013CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="99">
   <si>
     <t>pdb_id</t>
   </si>
@@ -159,9 +159,6 @@
     <t>ma-1dqrd</t>
   </si>
   <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
     <t>https://www.modelarchive.org/doi/10.5452/ma-c7d6n</t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>BHRF1 (2WH6)</t>
   </si>
   <si>
-    <t>EGFR (8HGO0</t>
-  </si>
-  <si>
     <t>Cas9 (4OO8)</t>
   </si>
   <si>
@@ -316,6 +310,30 @@
   </si>
   <si>
     <t>programmed cell death ligand 1</t>
+  </si>
+  <si>
+    <t>MGSHHHHHHSQDPMAYSTREILLALCIRDSRVHGNGTLHPVLELAARETPLRLSPEDTVVLRYHVLLEEIIERNSETFTETWNRFITHTEHVDLDFNSVFLEIFHRGDPSLGRALAWMAWCMHACRTLCCNQSTPYYVVDLSVRGMLEASEGLDGWIHQQGGWSTLIEDNIPG</t>
+  </si>
+  <si>
+    <t>EGFR (8HGO)</t>
+  </si>
+  <si>
+    <t>GSGHMDKKYSIGLAIGTNSVGWAVITDEYKVPSKKFKVLGNTDRHSIKKNLIGALLFDSGETAEATRLKRTARRRYTRRKNRILYLQEIFSNEMAKVDDSFFHRLEESFLVEEDKKHERHPIFGNIVDEVAYHEKYPTIYHLRKKLVDSTDKADLRLIYLALAHMIKFRGHFLIEGDLNPDNSDVDKLFIQLVQTYNQLFEENPINASGVDAKAILSARLSKSRRLENLIAQLPGEKKNGLFGNLIALSLGLTPNFKSNFDLAEDAKLQLSKDTYDDDLDNLLAQIGDQYADLFLAAKNLSDAILLSDILRVNTEITKAPLSASMIKRYDEHHQDLTLLKALVRQQLPEKYKEIFFDQSKNGYAGYIDGGASQEEFYKFIKPILEKMDGTEELLVKLNREDLLRKQRTFDNGSIPHQIHLGELHAILRRQEDFYPFLKDNREKIEKILTFRIPYYVGPLARGNSRFAWMTRKSEETITPWNFEEVVDKGASAQSFIERMTNFDKNLPNEKVLPKHSLLYEYFTVYNELTKVKYVTEGMRKPAFLSGEQKKAIVDLLFKTNRKVTVKQLKEDYFKKIEEFDSVEISGVEDRFNASLGTYHDLLKIIKDKDFLDNEENEDILEDIVLTLTLFEDREMIEERLKTYAHLFDDKVMKQLKRRRYTGWGRLSRKLINGIRDKQSGKTILDFLKSDGFANRNFMQLIHDDSLTFKEDIQKAQVSGQGDSLHEHIANLAGSPAIKKGILQTVKVVDELVKVMGRHKPENIVIEMARENQTTQKGQKNSRERMKRIEEGIKELGSQILKEHPVENTQLQNEKLYLYYLQNGRDMYVDQELDINRLSDYDVDAIVPQSFLKDDSIDNKVLTRSDKNRGKSDNVPSEEVVKKMKNYWRQLLNAKLITQRKFDNLTKAERGGLSELDKAGFIKRQLVETRQITKHVAQILDSRMNTKYDENDKLIREVKVITLKSKLVSDFRKDFQFYKVREINNYHHAHDAYLNAVVGTALIKKYPKLESEFVYGDYKVYDVRKMIAKSEQEIGKATAKYFFYSNIMNFFKTEITLANGEIRKRPLIETNGETGEIVWDKGRDFATVRKVLSMPQVNIVKKTEVQTGGFSKESILPKRNSDKLIARKKDWDPKKYGGFDSPTVAYSVLVVAKVEKGKSKKLKSVKELLGITIMERSSFEKNPIDFLEAKGYKEVKKDLIIKLPKYSLFELENGRKRMLASAGELQKGNELALPSKYVNFLYLASHYEKLKGSPEDNEQKQLFVEQHKHYLDEIIEQISEFSKRVILADANLDKVLSAYNKHRDKPIREQAENIIHLFTLTNLGAPAAFKYFDTTIDRKRYTSTKEVLDATLIHQSITGLYETRIDLSQLGGD</t>
+  </si>
+  <si>
+    <t>MELAALCRWGLLLALLPPGAASTQVCTGTDMKLRLPASPETHLDMLRHLYQGCQVVQGNLELTYLPTNASLSFLQDIQEVQGYVLIAHNQVRQVPLQRLRIVRGTQLFEDNYALAVLDNGDPLNNTTPVTGASPGGLRELQLRSLTEILKGGVLIQRNPQLCYQDTILWKDIFHKNNQLALTLIDTNRSRACHPCSPMCKGSRCWGESSEDCQSLTRTVCAGGCARCKGPLPTDCCHEQCAAGCTGPKHSDCLACLHFNHSGICELHCPALVTYNTDTFESMPNPEGRYTFGASCVTACPYNYLSTDVGSCTLVCPLHNQEVTAEDGTQRCEKCSKPCARVCYGLGMEHLREVRAVTSANIQEFAGCKKIFGSLAFLPESFDGDPASNTAPLQPEQLQVFETLEEITGYLYISAWPDSLPDLSVFQNLQVIRGRILHNGAYSLTLQGLGISWLGLRSLRELGSGLALIHHNTHLCFVHTVPWDQLFRNPHQALLHTANRPEDECVGEGLACHQLCARGHCWGPGPTQCVNCSQFLRGQECVEECRVLQGLPREYVNARHCLPCHPECQPQNGSVTCFGPEADQCVACAHYKDPPFCVARCPSGVKPDLSYMPIWKFPDEEGACQPCPINCTHSCVDLDDKGCPAEQRASPLTSIISAVVGILLVVVLGVVFGILIKRRQQKIRKYTMRRLLQEGGSENLYFQGGGSAQLEKELQALEKENAQLEWELQALEKELAQSNSLEVLFQ</t>
+  </si>
+  <si>
+    <t>MGDCDIEGKDGKQYESVLMVSIDQLLDSMKEIGSNCLNNEFNFFKRHICDANKEGMFLFRAARKLRQFLKMNSTGDFDLHLLKVSEGTTILLNCTGQVKGRKPAALGAAQPTKSLEENKSLKEQKKLNDLCFLKRLLQEIKTCWNKILMGTKEH</t>
+  </si>
+  <si>
+    <t>KIEEGKLVIWINGDKGYNGLAEVGKKFEKDTGIKVTVEHPDKLEEKFPQVAATGDGPDIIFWAHDRFGGYAQSGLLAEITPDKAFQDKLYPFTWDAVRYNGKLIAYPIAVEALSLIYNKDLLPNPPKTWEEIPALDKELKAKGKSALMFNLQEPYFTWPLIAADGGYAFKYGDIKDVGVDNAGAKAGLTFLVDLIKNKHMNADTDYSIAEAAFNKGETAMTINGPWAWSNIDTSKVNYGVTVLPTFKGQPSKPFVGVLSAGINAASPNKELAKEFLENYLLTDEGLEAVNKDKPLGAVALKSYEEELAKDPRIAATAENAAKGEIMPNIPQMSAFWYAVRTAVINAASGRQTVDEALKDAQTRITK</t>
+  </si>
+  <si>
+    <t>PD-L1 (4Z18)</t>
+  </si>
+  <si>
+    <t>MFTVTVPKDLYVVEYGSNMTIECKFPVEKQLDLAALIVYWEMEDKNIIQFVHGEEDLKVQHSSYRQRARLLKDQLSLGNAALQITDVKLQDAGVYRCMISYGGADYKRITVKVNAPYNKINQRILVVDPVTSEHELTCQAEGYPKAEVIWTSSDHQVLSGKTTTTNSKREEKLFNVTSTLRINTTTNEIFYCTFRRLDPEENHTAELVIPELPLAHPPNERT</t>
   </si>
 </sst>
 </file>
@@ -811,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -840,13 +858,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -881,13 +899,13 @@
         <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -917,19 +935,19 @@
     </row>
     <row r="3" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -959,102 +977,102 @@
     </row>
     <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>58</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>76</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -1062,119 +1080,157 @@
         <v>39</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="294.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="E14" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="K14" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="K15" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="K16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="10"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K22" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>